<commit_message>
Courts changements WBS avant présentation
</commit_message>
<xml_diff>
--- a/Livrables/18_03_2022_Presentation_R2.10/PlannificationPrevisionnelle.xlsx
+++ b/Livrables/18_03_2022_Presentation_R2.10/PlannificationPrevisionnelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Perso\Bureau\Travail\BUT-Info\S2\S2-05-Gestion_d_un_projet\Livrables\18_03_2022_Presentation_R2.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0991C33D-FE30-4449-A23F-93E3A8C6E30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D92B3C-BBA0-4F03-BCDB-2E405DAFBDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5250" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
   <si>
     <t>Choses à faire</t>
   </si>
@@ -218,6 +218,15 @@
   </si>
   <si>
     <t>Kepa, Alexandre</t>
+  </si>
+  <si>
+    <t>Très tardif et fait de manière peu homogène</t>
+  </si>
+  <si>
+    <t>Maquette de base bancale + collaboration difficile</t>
+  </si>
+  <si>
+    <t>Trop de détails (n'est pas une décomposition fonctionnelle)</t>
   </si>
 </sst>
 </file>
@@ -231,12 +240,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF212529"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -296,6 +299,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -341,65 +350,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,15 +687,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="56" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
@@ -699,717 +704,745 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="1">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="23">
         <f>AVERAGE(H4:H6)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="25">
+      <c r="C4" s="4"/>
+      <c r="D4" s="22">
         <v>44599</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="1">
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="1">
+      <c r="C5" s="4"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="1">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="23">
         <f>AVERAGE(H7:H9)</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="21">
         <v>44599</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16">
+      <c r="E7" s="21"/>
+      <c r="F7" s="21">
         <v>44599</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="21">
         <v>44604</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="1">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="1">
+      <c r="C9" s="4"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="1">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="23">
         <f>AVERAGE(H11:H14)</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>44602</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16">
+      <c r="E11" s="16"/>
+      <c r="F11" s="21">
         <v>44607</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="21">
         <v>44604</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="1">
+      <c r="C12" s="4"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="1">
+      <c r="C13" s="4"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <v>44630</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="8">
+      <c r="E14" s="16"/>
+      <c r="F14" s="13">
         <v>44605</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="6">
         <v>44634</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="1">
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="23">
         <f>AVERAGE(H16:H18)</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="17">
+      <c r="C16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="16">
         <v>44602</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="16">
+      <c r="E16" s="16"/>
+      <c r="F16" s="21">
         <v>44607</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="21">
         <v>44604</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="1">
+      <c r="C17" s="4"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="1">
+      <c r="C18" s="4"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="1">
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="23">
         <f>AVERAGE(H20:H23)</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="21">
         <v>44632</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="9">
+      <c r="E20" s="21"/>
+      <c r="F20" s="6">
         <v>44634</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="6">
         <v>44637</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="9">
+      <c r="C21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="6">
         <v>44640</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="6">
         <v>44676</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="9">
+      <c r="C22" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="6">
         <v>44638</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9">
+      <c r="E22" s="6">
+        <v>44682</v>
+      </c>
+      <c r="F22" s="6">
         <v>44661</v>
       </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="1">
+      <c r="G22" s="6">
+        <v>44682</v>
+      </c>
+      <c r="H22" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="6">
+        <v>44661</v>
+      </c>
+      <c r="E23" s="6">
+        <v>44632</v>
+      </c>
+      <c r="F23" s="6">
+        <v>44681</v>
+      </c>
+      <c r="G23" s="6">
+        <v>44680</v>
+      </c>
+      <c r="H23" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A24" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="23">
+        <f>AVERAGE(H25:H28)</f>
+        <v>0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="21">
+        <v>44683</v>
+      </c>
+      <c r="E25" s="21">
+        <v>44683</v>
+      </c>
+      <c r="F25" s="21">
+        <v>44691</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="23">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="23">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="23">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A23" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="6" t="s">
+    <row r="29" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A29" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="23">
+        <f>AVERAGE(H30:H33)</f>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="16">
+        <v>44691</v>
+      </c>
+      <c r="E30" s="21">
+        <v>44683</v>
+      </c>
+      <c r="F30" s="21">
+        <v>44701</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="23">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="23">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A32" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A33" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A34" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="16">
+        <v>44701</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="16">
+        <v>44706</v>
+      </c>
+      <c r="G34" s="10"/>
+      <c r="H34" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A35" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A36" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="9">
-        <v>44661</v>
-      </c>
-      <c r="E23" s="9">
-        <v>44632</v>
-      </c>
-      <c r="F23" s="9">
-        <v>44681</v>
-      </c>
-      <c r="G23" s="9">
-        <v>44680</v>
-      </c>
-      <c r="H23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A24" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="1">
-        <f>AVERAGE(H25:H28)</f>
+      <c r="C36" s="9"/>
+      <c r="D36" s="10">
+        <v>44707</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10">
+        <v>44722</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A25" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="16">
-        <v>44683</v>
-      </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="16">
-        <v>44691</v>
-      </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="1">
+    <row r="37" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A37" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A26" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="1">
+    <row r="38" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A38" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A27" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A28" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A29" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="1">
-        <f>AVERAGE(H30:H33)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A30" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="17">
-        <v>44691</v>
-      </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="16">
-        <v>44701</v>
-      </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A31" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A32" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A33" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A34" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="21">
-        <v>44701</v>
-      </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="21">
-        <v>44706</v>
-      </c>
-      <c r="G34" s="13"/>
-      <c r="H34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A35" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A36" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13">
-        <v>44707</v>
-      </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13">
-        <v>44722</v>
-      </c>
-      <c r="G36" s="13"/>
-      <c r="H36" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A37" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A38" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="1">
-        <v>0</v>
-      </c>
-    </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="2"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="20" t="s">
+      <c r="B40" s="14"/>
+      <c r="C40" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="15" t="s">
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="3">
         <f>AVERAGE(H29,H24,H19,H15,H10,H3,AVERAGE(H34:H38))</f>
-        <v>0.5357142857142857</v>
+        <v>0.64857142857142858</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="30">
+    <mergeCell ref="D20:E21"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="F25:F28"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="D16:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="G16:G18"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="C40:F40"/>
     <mergeCell ref="D34:D35"/>
@@ -1426,18 +1459,6 @@
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="D7:E9"/>
     <mergeCell ref="A24:G24"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="D16:E18"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="D20:E21"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="F25:F28"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="A29:G29"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:H38">
     <cfRule type="colorScale" priority="4">

</xml_diff>